<commit_message>
Set borders on all created cells and set text wrap on all created cells except date cells.
</commit_message>
<xml_diff>
--- a/template/table-only.xlsx
+++ b/template/table-only.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\diskstation\home\Drive\RubymineProjects\vh-events\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D9D7EFE-2D7D-4144-8602-F4A6C346CB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306E4388-50D4-4C4E-BB01-515C4B7791A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A40DE3AD-E031-4383-A1BB-AC0E2DF986DC}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -140,6 +140,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -478,18 +484,18 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="36.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="40.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="24" customHeight="1">
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -500,86 +506,86 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="41.25" customHeight="1">
+    <row r="2" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:3" ht="41.25" customHeight="1">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:3" ht="41.25" customHeight="1">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" ht="41.25" customHeight="1">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" ht="41.25" customHeight="1">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="25.5" customHeight="1">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>